<commit_message>
je jure j'ai push
</commit_message>
<xml_diff>
--- a/BDD.xlsx
+++ b/BDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\CY_TECH\ING2\S2\BDD\Projet\TAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0417901F-1A48-4297-89F6-A00CB71BB154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE656C-0514-4A27-8FD3-B99007753DFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BDD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
   <si>
     <t>Matériel</t>
   </si>
@@ -145,19 +145,10 @@
     <t>ticket_intervention</t>
   </si>
   <si>
-    <t>id_ticket</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>desription</t>
-  </si>
-  <si>
-    <t>license unitaire</t>
   </si>
   <si>
     <t>license_user</t>
@@ -421,6 +412,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,9 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -454,7 +443,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,26 +825,26 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -870,10 +861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,8 +879,8 @@
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
@@ -902,89 +893,69 @@
       <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="13"/>
       <c r="C4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="F4" s="13"/>
       <c r="G4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
       <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
       <c r="C6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
       <c r="C7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
       <c r="C8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
@@ -998,62 +969,52 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>44</v>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>43</v>
+      <c r="F11" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
       <c r="C12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="F12" s="13"/>
       <c r="G12" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
       <c r="C13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
       <c r="C14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="F3:F7"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1102,19 +1063,19 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="10" t="s">
@@ -1122,27 +1083,27 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1161,13 +1122,13 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -1175,11 +1136,11 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1182,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1232,7 +1193,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1202,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1211,7 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1259,7 +1220,7 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1275,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:K17"/>
+  <dimension ref="B1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,8 +1252,8 @@
     <col min="11" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1305,153 +1266,109 @@
       <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="F4" s="19"/>
       <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="18"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
       <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="F5" s="19"/>
       <c r="G5" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="18"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="19"/>
       <c r="G6" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
       <c r="C7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19"/>
       <c r="C8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23"/>
       <c r="C9" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>50</v>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
       <c r="C15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
       <c r="C16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="7" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="J3:J4"/>
+  <mergeCells count="3">
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="B3:B9"/>
   </mergeCells>

</xml_diff>